<commit_message>
New BOM generated and History folder deleted
</commit_message>
<xml_diff>
--- a/2022_03_17_STM32G031_SOIC8_Dev_Board/Project Outputs for STM32G031_SOIC8_Dev_Board/STM32G031_SOIC8_Dev_Board_rev_1.0.xlsx
+++ b/2022_03_17_STM32G031_SOIC8_Dev_Board/Project Outputs for STM32G031_SOIC8_Dev_Board/STM32G031_SOIC8_Dev_Board_rev_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javi_\GitHub\STM32G031_SOIC8_Dev_Board\2022_03_17_STM32G031_SOIC8_Dev_Board\Project Outputs for STM32G031_SOIC8_Dev_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7DC4CA6-307F-4328-8B3F-C01D06E25275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC386F50-CFF5-4AAC-B1F0-1FCCDECA2999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="2175" windowWidth="17355" windowHeight="17865" xr2:uid="{42199D99-5253-4D4D-B136-DB1BEE6C95D3}"/>
+    <workbookView xWindow="17580" yWindow="2175" windowWidth="17355" windowHeight="17865" xr2:uid="{A2BFBC63-71A8-4E92-9E50-B446CF3A6307}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32G031_SOIC8_Dev_Board_rev_1" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
     <t>SW1</t>
   </si>
   <si>
-    <t>830207390509</t>
+    <t>ASEKDV-32.768kHz-LC-T</t>
   </si>
   <si>
     <t>Crystal or Oscillator</t>
@@ -620,7 +620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A7D132-7DF0-4DEA-98D6-5EC091BDE69F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A43724-94BF-4831-9B1C-CF654DAE657D}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>